<commit_message>
updated react store configurations
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="154">
   <si>
     <t>Module Name</t>
   </si>
@@ -498,12 +498,15 @@
   <si>
     <t>BEM</t>
   </si>
+  <si>
+    <t>React Developer Tools</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -540,6 +543,13 @@
       <name val="Arial Unicode MS"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="21"/>
+      <color rgb="FF262626"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -568,7 +578,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -578,6 +588,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -897,8 +908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1025,10 +1036,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B4:M139"/>
+  <dimension ref="B4:M142"/>
   <sheetViews>
-    <sheetView topLeftCell="A122" workbookViewId="0">
-      <selection activeCell="B130" sqref="B130"/>
+    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
+      <selection activeCell="B146" sqref="B146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1655,6 +1666,11 @@
       </c>
       <c r="C139" t="s">
         <v>144</v>
+      </c>
+    </row>
+    <row r="142" spans="2:3" ht="27">
+      <c r="B142" s="7" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -1671,7 +1687,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>